<commit_message>
29032020 - Alter Estoque
</commit_message>
<xml_diff>
--- a/docs/Prof_Christiane/ESTOQUE/Análise de Eventos_ESTOQUE.xlsx
+++ b/docs/Prof_Christiane/ESTOQUE/Análise de Eventos_ESTOQUE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Master\docs\Prof_Christiane\ESTOQUE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre Queiroz\Desktop\Git Repositories\ope_ads\docs\Prof_Christiane\ESTOQUE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035A3D9E-817F-47D8-93E6-425CCBFB926D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Capacidades</t>
   </si>
@@ -58,19 +59,12 @@
     <t>Temporal</t>
   </si>
   <si>
-    <t>Extem-por
-âneo</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
     <t>Fornecedor realiza a entrega do pedido.</t>
   </si>
   <si>
-    <t>x(1)</t>
-  </si>
-  <si>
     <t>FB</t>
   </si>
   <si>
@@ -80,35 +74,29 @@
     <t>Fornecedor não entrega o pedido.</t>
   </si>
   <si>
-    <t>Estabelecimento gera relatórios.</t>
-  </si>
-  <si>
     <t>Gerenciar reposição</t>
   </si>
   <si>
-    <t>Gerar relatórios</t>
-  </si>
-  <si>
     <t>Gerenciar produtos</t>
-  </si>
-  <si>
-    <t>Estabelecimento descarta produtos.</t>
   </si>
   <si>
     <t>Gerencia condição
 dos produtos.</t>
   </si>
   <si>
-    <t>Estabelecimento gerencia os produtos.</t>
-  </si>
-  <si>
-    <t>Estabelecimento gera pedido de troca.</t>
+    <t>Extemporâneo</t>
+  </si>
+  <si>
+    <t>Estoquista gerencia os produtos.</t>
+  </si>
+  <si>
+    <t>Estoquista descarta produtos.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,14 +165,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -240,24 +222,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -301,8 +270,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -314,12 +283,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -608,11 +571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -623,7 +586,7 @@
     <col min="4" max="4" width="40.140625" style="12" customWidth="1"/>
     <col min="5" max="6" width="12.140625" style="5" customWidth="1"/>
     <col min="7" max="9" width="11.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -668,24 +631,24 @@
         <v>8</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="6"/>
@@ -696,35 +659,35 @@
     <row r="4" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="13">
         <v>2</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="13">
         <v>3</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -732,21 +695,21 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>22</v>
+    <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="13">
         <v>4</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -754,58 +717,15 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="13">
-        <v>5</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="13">
-        <v>6</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>